<commit_message>
Agregando la nueva interfaz con los logos
</commit_message>
<xml_diff>
--- a/assets/Example.xlsx
+++ b/assets/Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabia\Desktop\acl-manager\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFA8B1D-B643-4BA4-9DD4-BD81C1394961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1675F485-FE88-4680-B6FF-BECF3DB6AAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1200" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -207,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,7 +491,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,8 +542,8 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>3</v>

</xml_diff>